<commit_message>
Exception and Fault samples added
</commit_message>
<xml_diff>
--- a/DotNet.xlsx
+++ b/DotNet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Serialization</t>
   </si>
@@ -324,12 +324,150 @@
 Dispatcher calls this method when it doesn't find a matching action
 only one method per contact can be annotated this way</t>
   </si>
+  <si>
+    <t>Exceptions and Faults</t>
+  </si>
+  <si>
+    <t>Moving between two</t>
+  </si>
+  <si>
+    <t>FaultException &amp; FaultException&lt;T&gt;</t>
+  </si>
+  <si>
+    <t>Global exception Handling</t>
+  </si>
+  <si>
+    <t>Handling Exceptions on the client</t>
+  </si>
+  <si>
+    <t>Throwing &amp; Cathing faults [FaultContract]</t>
+  </si>
+  <si>
+    <t>IErrorHandler</t>
+  </si>
+  <si>
+    <t>Exceptions are technology specific and hence they cannot cross the service boundry, SOAP defines a standard representations ofor eror referred to as SOAp FAULTS. Wcf knows how to translate between the two.</t>
+  </si>
+  <si>
+    <t>.net Service (throw new Exception())---&gt; Soap (fault) std representation---&gt; Java Client(catch(Exception e)</t>
+  </si>
+  <si>
+    <t>&lt;s:Envelope  ……………………&gt;
+   &lt;s:Body&gt;
+   &lt;fault&gt;
+      &lt;faultcode&gt;s:Client&lt;/faultcode&gt;
+     &lt;faultstring xml:lang="en-US&gt;-something bad happened&lt;/fault&gt;
+    &lt;detail&gt;Anything you want goes here&lt;/detail&gt;
+   &lt;/fault&gt;
+  &lt;/Body&gt;
+&lt;/s:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>&lt;env:Envelope  ……………………&gt;
+   &lt;env:Body&gt;
+   &lt;env:fault&gt;
+      &lt;env:code&gt;
+           &lt;env:Value&gt;env:Sender &lt;env:Value&gt;
+           &lt;envSub:code&gt;&lt;env:Value&gt;error:myerror &lt;env:Value&gt;&lt;/env:code&gt;/envSub:code&gt;
+     &lt;/env:code&gt;
+     &lt;env:Reason&gt;
+        &lt;env:Text xml:lang="en-US"&gt;Processing Error&lt;/env:Text&gt;
+     &lt;/env:Reason&gt;
+    &lt;env:Details&gt;...... &lt;/env:Details&gt;
+   &lt;/env:fault&gt;
+  &lt;/env:Body&gt;
+&lt;/env:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>Soap faults 1.1 or 1.2 whatever is sent is base on the bindings that u select</t>
+  </si>
+  <si>
+    <t>WCF Builtin Exception Handling</t>
+  </si>
+  <si>
+    <t>When a service op produces an exception, the dispatcher catches it and transmit a SOAP fault to the client, it doesn't take down the process but it might fault the channel.
+It sends back the following info to the client and that depends on what type of exception is
+-if FaultException(or a derivate) all details are transmitted
+-if it is anything esle a generic fault is transmitted by default, the design is to prevent undesired system disclosure.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Generic SOAP fault produced by a non-Fault Exception
+&lt;faultcode&gt;a:InternalServiceFault&lt;/faultcode&gt;: Thsta a special faultcode defined by wcf to indicate that something went wrong within the service and we are not going to give any details
+To include exception details in the fault, use either [ServiceBehavior] or &lt;serviceDebug&gt; to enable, useful for debugging purpose and not recommended in production.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[ServiceBehavior(InstanceContextMode = InstanceContextMode.Single, IncludeExceptionDetailInFaults =true)]
+public class EvalService : IEvalService</t>
+    </r>
+  </si>
+  <si>
+    <t>You can throw a SOAP fault using the FaultException calsss, you can specify reason and code when u create it, when we do this the fault details do indeed travel to the client. No need for IncludeExceptionDetailsInFault.
+The faults will be re-thrown as a FaultException on the client side, clients can simply use a traditional try/catch block to handle it. The faultcode/reason will be available within the instance</t>
+  </si>
+  <si>
+    <t>FaultException derives form Exception class, but then faultcode and fault reason will not be available if instead of faultException only Exception is used in the catch block.</t>
+  </si>
+  <si>
+    <t>FaultException&lt;T&gt;</t>
+  </si>
+  <si>
+    <t>FaultException produces a simple SOAP fault with code/reason, makes difficut for the clients to distinguish between different errors. A better techniques is to throw a typed fault. Define a data cntract type for fault information, throw the typed fauult with FaultException&lt;T&gt;</t>
+  </si>
+  <si>
+    <t>svctraceviewer to view tracelog
+configure the AppConfig of the host application --&gt;Diagnostics--&gt; enable message logging</t>
+  </si>
+  <si>
+    <t>You advertise fault types via [FaultContract] your service contracts
+use[FaultContract] to specify each fault type it can throw, the detail type must be serializable with DataContractSerializer. Cannot use [FaultContract] on onew-way operations.</t>
+  </si>
+  <si>
+    <t>Wcf makes it possible to implement a global exception handler, that allows you to shield clients from all undeclared exceptions, allows to perform a mapping to your declared fault types, allows to centralize error looging/notification logic. This all done thru IErrorHandler interface</t>
+  </si>
+  <si>
+    <t>ProvideFault and HandleError
+PE:- is called immediately after an exception is thrown and allows to generate a custom fault message.
+HandleError is called on a separate thread after return to client that allows to perform more time consumeing error logging techniques.</t>
+  </si>
+  <si>
+    <t>You inject your Ierrorhandler implementation using behavior
+-Implemet a service behaviour derived from IserviceBehavior and add it to the ChannelIDispatcher's ErrorHandlersproperty
+You can apply your behavior to the WCF runtime a few different ways
+-Add it explicitly to the ServiceHost.Description.Behaviors property
+Make the behaviuor an attribute an add the attribute to the service
+Define a behavior extension element and add via configiration</t>
+  </si>
+  <si>
+    <t>FaultException&lt;T&gt;- FautException--CommunicationException--TimeOutExceptions
+FaultException is derived from CommunicationException</t>
+  </si>
+  <si>
+    <t>When a client channel receives based on the type of fault and type of channel
+-When a sessionful channels receive InternalServiceFault the channel enters a faulted state
+-Once the client channel has faulted you can only Abort
+check the channels State property to be sure
+FaultException-derived types never fault the client channel.</t>
+  </si>
+  <si>
+    <t>You will be tempted to wrap the client channel in a using statement, doing so automates the call to calose when leaving scope.
+Close can also throw communication/timeout exceptions, Close always thorws an exception on faulted channels.
+-Either don't use the using statement or override Dispose in a partial class.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +477,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -381,11 +526,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -850,7 +998,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,6 +1101,9 @@
       <c r="B11" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -961,14 +1112,123 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="79.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="214.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WCF Security Samples added
</commit_message>
<xml_diff>
--- a/DotNet.xlsx
+++ b/DotNet.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Serialization" sheetId="1" r:id="rId1"/>
     <sheet name="ServiceContract" sheetId="2" r:id="rId2"/>
     <sheet name="ExceptionFaults" sheetId="3" r:id="rId3"/>
+    <sheet name="Security" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>Serialization</t>
   </si>
@@ -461,6 +462,252 @@
     <t>You will be tempted to wrap the client channel in a using statement, doing so automates the call to calose when leaving scope.
 Close can also throw communication/timeout exceptions, Close always thorws an exception on faulted channels.
 -Either don't use the using statement or override Dispose in a partial class.</t>
+  </si>
+  <si>
+    <t>WCF provides 3 imp security features (CIA), security is on by default in almost all the bindings. You configure transport  vs message using security mode. You configure authentication vis the client credentials type.
+WCF provieds numerous authorization options- Impersonation, Role based Access control (RBAC) and Service authorization behavior</t>
+  </si>
+  <si>
+    <t>Confidentiality</t>
+  </si>
+  <si>
+    <t>Encrypting msg mitigates eavesdroping attacks</t>
+  </si>
+  <si>
+    <t>Integrity</t>
+  </si>
+  <si>
+    <t>Signing msg mitigates tampering and replay attacks</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Proof of identity mitigates spoofing and impersonation attacks</t>
+  </si>
+  <si>
+    <t>ServiceSecurityContext calls is used to represent the information about the incoming caller</t>
+  </si>
+  <si>
+    <t>cmd promp
+runas  /user:saurabh "path to exe" and enter password sj@01012017</t>
+  </si>
+  <si>
+    <t>either netTcp or WcfHttp binding, security context flows for Authentication by default</t>
+  </si>
+  <si>
+    <t>Decisions to be made:</t>
+  </si>
+  <si>
+    <t>1.Protection level required by ur services- should the data be signed, encrypted or both
+2. Transport vs message security on bindings- can also use a hybrid of the two
+3. Authentication or who are you- choose the type of credentials you want the cleint to use and wcf will pick the appropriate authetication protocol
+4. Authorization: what are you allowed-Impersonate the caller letteing someone else handle authorization, provide your authorization management</t>
+  </si>
+  <si>
+    <t>Protection Levels</t>
+  </si>
+  <si>
+    <t>The developer of a service doesn't ultimately control how it is exposed, so what if the host application exposes unsecure endpoints. Hence the developer can set the required protection levels on the contracts. The host will fail if the required protection level isn't met by the endpoint. You can set the protection level at different scopes:
+-On a particular msg
+-On individual operation and fault contracts
+-On service contract</t>
+  </si>
+  <si>
+    <t>[MessageContract(ProtectionLevel=ProtectionLevel.EncryptAndSign)]
+[ServiceContract(ProtectionLevel=ProtectionLevel.Sign)]
+[OperationContract(ProtectionLevel=ProtectionLevel.None)]</t>
+  </si>
+  <si>
+    <t>BasicHttpBinding: By default doesn't provide encryption and sign
+wsHttpBinding: Message is signed and encrypetd by default at the message layer and could be seen in traceviewer
+netTcp: the message is secured (signed and encrypted) at the transport level and cannot be seen in traceviewer as encrypted as once the message has beenreceived it is already decrypted.</t>
+  </si>
+  <si>
+    <t>By default security is enabled on most of the bindings, however if you are involved in deciding how those works you can configure following:-
+Security Mode- Transport, Message or Mixed
+Client Credential Type: UserName, Cerificate, Windows, IssuedToken ( This determines what authentical protocol is used by wcf at runtime)</t>
+  </si>
+  <si>
+    <t>Security in Bindings
+Deermines how security protocol is implemented at runtime</t>
+  </si>
+  <si>
+    <t>1. wsHttpBinding:  securitymode= transport, --means SSL will be used(https), clientcredentialtype=windows --means that client needs to transmit windows credentials
+2. wsHttpBinding: securitymode= message -default for wshttpbindings, clientcredentialtype="UserName" (username and pwd is supplied in soap message). with this wcf service also requires that service be configured with x.509 certificates
+3.Mode=TransportwithMessageCredential and clientcredentialtype=IssueToken this means that service will use SSL and tranport will be Https and WsHttp header will contain issued token which will be a SAML token</t>
+  </si>
+  <si>
+    <t>Transport Security</t>
+  </si>
+  <si>
+    <t>Each transport typically has abuilt in security layer that you can use [Provides point2point security between nodes]
+-Http with SSL
+-TCP/NP using kerberos or NTLM
+-MSMQ using certificate 
+Problematic if architecture requires intermediaries</t>
+  </si>
+  <si>
+    <t>Pros:
+Mature well understood security model, better performance
+Cons:-
+Constrain the type of clientcredential
+get only point-to-point authentication and not ene-to end authentication</t>
+  </si>
+  <si>
+    <t>Message Security</t>
+  </si>
+  <si>
+    <t>With msg based sec we are essentially taking all the authenticationinformation that used to exist up within the transport headers and we are shoving it down into the actual SOAP message. We put that information into the SOAP header section using the WS Security Header elements as defined by that specification. so the security information is within the SOAP envelope.
+-Msg sec pushes authentication down into the soap header
+Provides same security features as transport security, but in a transport neutral way (pushes security into SOAP msg)
+Provides an end to end security solution across all nodes</t>
+  </si>
+  <si>
+    <t>Pros:
+Supports wide variety of credentials,Largely independent of transport
+support end-to-end authentication,Multiple wcf extensibilty hooks
+Cons
+Newer isn't alwy better for security
+WS* isn't as broadly adopted as SSL
+Pref can be significantly worse</t>
+  </si>
+  <si>
+    <t>Speed &amp; Maturity of Transport security and Flexibility of Client credential types embedded in msg
+Trsnport security typically supplied SSL, authentices service to a client via services certificate, sign &amp; encrypt payload
+WS-Security header holds client credential, opens up many options for credential format
+secured pipe thru which message can be passed with client credential types</t>
+  </si>
+  <si>
+    <t>TransportwithMsgCredential</t>
+  </si>
+  <si>
+    <t>Credentials Format</t>
+  </si>
+  <si>
+    <t>ClientCredentialType:
+selects the type of credentials the client must present
+Implictly dictates the type of credential the server must possess
+a certificate for the service endpoint is almost always needed.</t>
+  </si>
+  <si>
+    <t>CCT                                 Implied Service credential Type
+-----------------            ---------------------------------------                                  
+None                            Certificate (Optional)
+UserName                 Certificate (service needs to be configured with certificate)
+Certificate                 Certificate
+Windows                   Windows
+IssuedToken            Certificate
+When the client send the information over the wire that information needs to be signed and encrypted sp that no one can tamper with or read it along the way</t>
+  </si>
+  <si>
+    <t>Authentication in std Bindings</t>
+  </si>
+  <si>
+    <t>Open mmc-&gt;certificates-&gt;Localcomputer, currentuser
+copy certificate localhost from localcomputer-Personal-certificate  to currentuser--&gt;TrusterRootCertification Authority-certificate</t>
+  </si>
+  <si>
+    <t>Binding                                                          Transport                                          Message                                  Default ClientCredentialType
+------------------------------                        -------------------                             ------------                                 -------------------------------------
+BasicHttpBindings                                     Supported                                       Supported                               None
+WsHttp                                                           Supported                                       Default                                     Windows
+WsDualHttp                                                  Supported                                       Default                                     Windows
+NetTcp                                                            Default                                             Supported                               Windows
+NetNamedPipe                                           Default                                            Supported                                Windows
+NetMsmq                                                       Default                                             Supported                                Windows</t>
+  </si>
+  <si>
+    <t>Security call context</t>
+  </si>
+  <si>
+    <t>The incoming caller will be populated in the security call context object
+Every secure operation has a ServiceSecurityContext object, ServiceSecurityContext.Current
+OperationContext.ServiceSecurityContext</t>
+  </si>
+  <si>
+    <t>The context object provides with info about the calle
+-Use PrimaryIdentity or WindowsIdentity to access the Iidentity object
+IsAnonymous will tell if it was an anonymous call
+OperationContext ctx = OperationContext.Current
+ServiceSecurityContext sctx = ctx.ServiceSecurityContext 
+if(null==sctx) throw AccessDeniedFault();
+IIdentity id = stcx.PrimaryIdentity;
+auditOperation("Approve" , id.Name);</t>
+  </si>
+  <si>
+    <t>Authorization Options</t>
+  </si>
+  <si>
+    <t>RBAC- writing code against that incomming caller information (explicit authorization logic)
+-Windows groups a simple option (use Iprincipal), can if IsInRole().
+-Use an ASP.Net role provider
+-PrincipalPermission works reasonably well and can use this attribute to make it declarative</t>
+  </si>
+  <si>
+    <t>ServiceAuthorization behavior does the same thing but it happens earlier in theWCF pipeline, before u reach the code. 
+-Decision based on SOAP action and client identity
+Fires earlier than PrincipalPermission
+Hoists authorization logic out of service implementations</t>
+  </si>
+  <si>
+    <t>All of the authorization logic is now decoupled from service implementation, because it is now found within a behaviour and that behavior can be declaratively applied to multiple service implementations simply through a config file entry. Requse and the ability to add logic in a more declarative fashion to your service.</t>
+  </si>
+  <si>
+    <t>Impersonation
+Only an option w/windos creds
+Use WindowsIdentity.Impersonate or [OperationBehavior]</t>
+  </si>
+  <si>
+    <t>Impersonation is a Windows feature, must be using Windows authn for this to work, easy to get this working for local resources, trickier for remote resources (required delegation)
+Temprarily take on the client's identity,  u r passing the  authorization problem to a system behind u. Great when u r accessing existing secure resources, can eliminate the need for u to implement autz in ur app.</t>
+  </si>
+  <si>
+    <t>Groups/Roles/Claims</t>
+  </si>
+  <si>
+    <t>Windows group can be used directly for authorization
+Thread.CurrentPrincipal.IsInRole("mydoamin\mygroup")
+[PrinciplaPermission(…,Role=mydoamin\mygroup")]--hard to deploye if domain/mcname are gard coded</t>
+  </si>
+  <si>
+    <t>Can use AzMan or ASP.Net role provider
+Thread.CurrentPrincipal.IsInRole("MyRole")
+[PrinciplaPermission(…,Role="MyRole")]
+Each application has its own roles no name collision</t>
+  </si>
+  <si>
+    <t>To prepare for federation scenarios start thinking about claims
+Claims are a superset of group and roles</t>
+  </si>
+  <si>
+    <t>Federation &amp; Claims</t>
+  </si>
+  <si>
+    <t>Federations allows you to rely on identity information from trusted partners or identity providers
+-No need to provision accounts for users (reduces costs)
+-Security tokens for usrs consist of a signed set of claims-each claim is a statement about the user
+signaures tells you who is making the statements. (basically the identity provider)
+Structure of a claim is very simple- Uri indicates type of claim, name of claim and Value of claim.</t>
+  </si>
+  <si>
+    <t>Claim based authorization</t>
+  </si>
+  <si>
+    <t>Claims are the most general purpose authorization mechanism
+-supports windows groups, roles, federated identity scenarios and Cardspace
+Each authenticated client presents a set of claims
+-services can enumerate claim and make authorization decision, available via ServiceSecurityContext.AuthorizationContext</t>
+  </si>
+  <si>
+    <t>Authorization Behaior</t>
+  </si>
+  <si>
+    <t>Dest to do authz as early as possible in the pipeline, why decrypt the message body if you are just going to reject it, why marshal the message etc
+Service Authorization behavior allows you to do this
+-Must derive a class from ServiceAuthorizationManager, given SOAP action and security context return a boolean indicating whether the user may perform the action
+Compare this to using [PrincipalPermission] or IsInRole
+These techniques can also happen after message is unmarshalled, using behavior also helps you to isolate autorization logic from business logic which is a good idea.</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1231,4 +1478,231 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="125.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="111.42578125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>